<commit_message>
Version evolucionada con generacion de excel,tocado
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>bloque</t>
   </si>
@@ -44,7 +44,7 @@
     <t>REF</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>-</t>
@@ -53,7 +53,7 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Total REF</t>
@@ -62,100 +62,112 @@
     <t>ROWS</t>
   </si>
   <si>
-    <t>11</t>
+    <t>13</t>
   </si>
   <si>
     <t>Total NEW</t>
   </si>
   <si>
-    <t>12</t>
+    <t>16</t>
   </si>
   <si>
     <t>Total (NEW-REF)</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>23.1%</t>
+  </si>
+  <si>
+    <t>Quality global</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (exact matches)</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>33.3%</t>
+  </si>
+  <si>
+    <t>4_BR,NULL_GR</t>
+  </si>
+  <si>
+    <t>NO MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (match not identical)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>66.7%</t>
+  </si>
+  <si>
+    <t>1_US,2_ES,8_BR,9_AN</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>1:0 (only in reference)</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>45.5%</t>
+  </si>
+  <si>
+    <t>10_GR,3_MX,4_FR,5_FR,7_PT</t>
+  </si>
+  <si>
+    <t>0:1 (only in new)</t>
+  </si>
+  <si>
+    <t>25.0%</t>
+  </si>
+  <si>
+    <t>6_DE,7_NULL</t>
+  </si>
+  <si>
+    <t>DUPS</t>
+  </si>
+  <si>
+    <t>duplicates (both)</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>16.7%</t>
+  </si>
+  <si>
+    <t>NULL_GR</t>
+  </si>
+  <si>
+    <t>duplicates (ref)</t>
+  </si>
+  <si>
     <t>9.1%</t>
-  </si>
-  <si>
-    <t>Quality global</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (exact matches)</t>
-  </si>
-  <si>
-    <t>BOTH</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>20.0%</t>
-  </si>
-  <si>
-    <t>4_BR</t>
-  </si>
-  <si>
-    <t>NO MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (match not identical)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>80.0%</t>
-  </si>
-  <si>
-    <t>1_US,2_ES,8_BR,9_AN</t>
-  </si>
-  <si>
-    <t>GAP</t>
-  </si>
-  <si>
-    <t>1:0 (only in reference)</t>
-  </si>
-  <si>
-    <t>50.0%</t>
-  </si>
-  <si>
-    <t>10_GR,3_MX,4_FR,5_FR,7_PT</t>
-  </si>
-  <si>
-    <t>0:1 (only in new)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>28.6%</t>
-  </si>
-  <si>
-    <t>6_DE,7_NULL</t>
-  </si>
-  <si>
-    <t>DUPS</t>
-  </si>
-  <si>
-    <t>duplicates (both)</t>
-  </si>
-  <si>
-    <t>duplicates (ref)</t>
-  </si>
-  <si>
-    <t>10.0%</t>
   </si>
   <si>
     <t>5_FR</t>
@@ -387,154 +399,154 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade un tipo de dato numerico BigDecimal genrico para que los datos numericos sean agnosticos y un fix en TableComprator
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>bloque</t>
   </si>
@@ -44,7 +44,7 @@
     <t>REF</t>
   </si>
   <si>
-    <t>11</t>
+    <t>10</t>
   </si>
   <si>
     <t>-</t>
@@ -98,85 +98,76 @@
     <t>BOTH</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>14.3%</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>NO MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (match not identical)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>85.7%</t>
+  </si>
+  <si>
+    <t>1,2,4,7,8,9</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>1:0 (only in reference)</t>
+  </si>
+  <si>
+    <t>30.0%</t>
+  </si>
+  <si>
+    <t>10,3,5</t>
+  </si>
+  <si>
+    <t>0:1 (only in new)</t>
+  </si>
+  <si>
+    <t>12.5%</t>
+  </si>
+  <si>
+    <t>DUPS</t>
+  </si>
+  <si>
+    <t>duplicates (both)</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>33.3%</t>
-  </si>
-  <si>
-    <t>4_BR,NULL_GR</t>
-  </si>
-  <si>
-    <t>NO MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (match not identical)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>66.7%</t>
-  </si>
-  <si>
-    <t>1_US,2_ES,8_BR,9_AN</t>
-  </si>
-  <si>
-    <t>GAP</t>
-  </si>
-  <si>
-    <t>1:0 (only in reference)</t>
+    <t>28.6%</t>
+  </si>
+  <si>
+    <t>4,NULL</t>
+  </si>
+  <si>
+    <t>duplicates (ref)</t>
+  </si>
+  <si>
+    <t>10.0%</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>45.5%</t>
-  </si>
-  <si>
-    <t>10_GR,3_MX,4_FR,5_FR,7_PT</t>
-  </si>
-  <si>
-    <t>0:1 (only in new)</t>
-  </si>
-  <si>
-    <t>25.0%</t>
-  </si>
-  <si>
-    <t>6_DE,7_NULL</t>
-  </si>
-  <si>
-    <t>DUPS</t>
-  </si>
-  <si>
-    <t>duplicates (both)</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>16.7%</t>
-  </si>
-  <si>
-    <t>NULL_GR</t>
-  </si>
-  <si>
-    <t>duplicates (ref)</t>
-  </si>
-  <si>
-    <t>9.1%</t>
-  </si>
-  <si>
-    <t>5_FR</t>
-  </si>
-  <si>
     <t>duplicates (new)</t>
-  </si>
-  <si>
-    <t>4_BR,6_DE</t>
   </si>
 </sst>
 </file>
@@ -445,16 +436,16 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
         <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -462,7 +453,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -474,64 +465,64 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -543,10 +534,10 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
README actualizado para detalle de duplicados
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>bloque</t>
   </si>
@@ -44,7 +44,7 @@
     <t>REF</t>
   </si>
   <si>
-    <t>10</t>
+    <t>9</t>
   </si>
   <si>
     <t>-</t>
@@ -53,7 +53,7 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>8</t>
+    <t>7</t>
   </si>
   <si>
     <t>Total REF</t>
@@ -68,82 +68,79 @@
     <t>Total NEW</t>
   </si>
   <si>
-    <t>16</t>
+    <t>15</t>
   </si>
   <si>
     <t>Total (NEW-REF)</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>15.4%</t>
+  </si>
+  <si>
+    <t>Quality global</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (exact matches)</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>33.3%</t>
+  </si>
+  <si>
+    <t>1,NULL</t>
+  </si>
+  <si>
+    <t>NO MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (match not identical)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>66.7%</t>
+  </si>
+  <si>
+    <t>2,4,7,8</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>1:0 (only in reference)</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>23.1%</t>
-  </si>
-  <si>
-    <t>Quality global</t>
+    <t>10,3,5</t>
+  </si>
+  <si>
+    <t>0:1 (only in new)</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>10.0%</t>
-  </si>
-  <si>
-    <t>MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (exact matches)</t>
-  </si>
-  <si>
-    <t>BOTH</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>28.6%</t>
-  </si>
-  <si>
-    <t>1,NULL</t>
-  </si>
-  <si>
-    <t>NO MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (match not identical)</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>71.4%</t>
-  </si>
-  <si>
-    <t>2,4,7,8,9</t>
-  </si>
-  <si>
-    <t>GAP</t>
-  </si>
-  <si>
-    <t>1:0 (only in reference)</t>
-  </si>
-  <si>
-    <t>30.0%</t>
-  </si>
-  <si>
-    <t>10,3,5</t>
-  </si>
-  <si>
-    <t>0:1 (only in new)</t>
-  </si>
-  <si>
-    <t>12.5%</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>14.3%</t>
   </si>
   <si>
     <t>DUPS</t>
@@ -156,6 +153,12 @@
   </si>
   <si>
     <t>duplicates (ref)</t>
+  </si>
+  <si>
+    <t>22.2%</t>
+  </si>
+  <si>
+    <t>1,5</t>
   </si>
   <si>
     <t>duplicates (new)</t>
@@ -381,76 +384,76 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
         <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -459,67 +462,67 @@
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -528,7 +531,7 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadida lectura de csv y parquet, con el fin de ser agnostico a las fuentes de datos.
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>bloque</t>
   </si>
@@ -44,7 +44,7 @@
     <t>REF</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>-</t>
@@ -53,96 +53,99 @@
     <t>NEW</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Total REF</t>
+  </si>
+  <si>
+    <t>ROWS</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Total NEW</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Total (NEW-REF)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>23.1%</t>
+  </si>
+  <si>
+    <t>Quality global</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10.0%</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (exact matches)</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
-    <t>Total REF</t>
-  </si>
-  <si>
-    <t>ROWS</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Total NEW</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Total (NEW-REF)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>15.4%</t>
-  </si>
-  <si>
-    <t>Quality global</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (exact matches)</t>
-  </si>
-  <si>
-    <t>BOTH</t>
+    <t>28.6%</t>
+  </si>
+  <si>
+    <t>1,NULL</t>
+  </si>
+  <si>
+    <t>NO MATCH</t>
+  </si>
+  <si>
+    <t>1:1 (match not identical)</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>71.4%</t>
+  </si>
+  <si>
+    <t>2,4,7,8,9</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>1:0 (only in reference)</t>
+  </si>
+  <si>
+    <t>30.0%</t>
+  </si>
+  <si>
+    <t>10,3,5</t>
+  </si>
+  <si>
+    <t>0:1 (only in new)</t>
+  </si>
+  <si>
+    <t>12.5%</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>33.3%</t>
-  </si>
-  <si>
-    <t>1,NULL</t>
-  </si>
-  <si>
-    <t>NO MATCH</t>
-  </si>
-  <si>
-    <t>1:1 (match not identical)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>66.7%</t>
-  </si>
-  <si>
-    <t>2,4,7,8</t>
-  </si>
-  <si>
-    <t>GAP</t>
-  </si>
-  <si>
-    <t>1:0 (only in reference)</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>10,3,5</t>
-  </si>
-  <si>
-    <t>0:1 (only in new)</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>14.3%</t>
-  </si>
-  <si>
     <t>DUPS</t>
   </si>
   <si>
@@ -153,12 +156,6 @@
   </si>
   <si>
     <t>duplicates (ref)</t>
-  </si>
-  <si>
-    <t>22.2%</t>
-  </si>
-  <si>
-    <t>1,5</t>
   </si>
   <si>
     <t>duplicates (new)</t>
@@ -384,76 +381,76 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -462,67 +459,67 @@
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -531,7 +528,7 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
activar test main2 en push y pull request
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -77,7 +77,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>15.4%</t>
+    <t>15,4%</t>
   </si>
   <si>
     <t>Quality global</t>
@@ -86,7 +86,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>0.0%</t>
+    <t>0,0%</t>
   </si>
   <si>
     <t>MATCH</t>
@@ -101,7 +101,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>33.3%</t>
+    <t>33,3%</t>
   </si>
   <si>
     <t>1,NULL</t>
@@ -116,7 +116,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>66.7%</t>
+    <t>66,7%</t>
   </si>
   <si>
     <t>2,4,7,8</t>
@@ -140,7 +140,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>14.3%</t>
+    <t>14,3%</t>
   </si>
   <si>
     <t>DUPS</t>
@@ -155,7 +155,7 @@
     <t>duplicates (ref)</t>
   </si>
   <si>
-    <t>22.2%</t>
+    <t>22,2%</t>
   </si>
   <si>
     <t>1,5</t>

</xml_diff>